<commit_message>
clarify the training process.
</commit_message>
<xml_diff>
--- a/model list.xlsx
+++ b/model list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA63F893-B8A0-4462-8911-07FDE78B96C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F623F-BF6E-4950-A2A9-449F4148E6E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
   <si>
     <t>phase</t>
   </si>
@@ -34,9 +34,6 @@
     <t>train_cw_aug</t>
   </si>
   <si>
-    <t>base model</t>
-  </si>
-  <si>
     <t>train_cw_aug_gbvs</t>
   </si>
   <si>
@@ -173,16 +170,161 @@
   </si>
   <si>
     <t>这个好像还不是第一步，这个也需要初始化</t>
+  </si>
+  <si>
+    <t>test_Wildcat_WK_hd_compf_multiscale_cw_sa_sp</t>
+  </si>
+  <si>
+    <t>先得到_fixf_sp或者_fixf_nob的weight，再训练整个model</t>
+  </si>
+  <si>
+    <t>看起来  又好像只是为了noGrid, noobj, nopsal这几个特殊的baseline的</t>
+  </si>
+  <si>
+    <t>train_alt_alpha_sa_new</t>
+  </si>
+  <si>
+    <t>new_fixf</t>
+  </si>
+  <si>
+    <t>train_cw_aug_sa_new</t>
+  </si>
+  <si>
+    <t>没有att_soft_score来生成A‘，但是用relation预测了class来融合cw_map得到sal_map</t>
+  </si>
+  <si>
+    <t>base model; emm 这个好像是第一步呀</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA16_alt_2_compf_cls_att_gd_nf4_norm</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA16_alt_2_compf_cls_att_gd_nf4_normTrue_hb_50_aug7_gbvs_0.5_thm_rf0.1 _hth0.1_2_ms4_kmax1_kminNone_a0.7_M4_fFalse_dlTrue_one3_224_epoch11.pt'</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA{}_alt_2_compf_cls_att_gd_nf4_norm{}_hb_{}_aug7_{}_{}_thm_rf{}_hth{}_2_ms4_kmax{}_kmin{}_a{}_M{}_f{}_dl{}_one3_224</t>
+  </si>
+  <si>
+    <t>train_cw_alt_alpha (model_name)</t>
+  </si>
+  <si>
+    <t>0-2</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>train_cw_alt_alpha (checkpoint)</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA16_compf_cls_att_gd_nf4_normTrue_hb_50_aug7_bms_thm_rf0.1_hth0.1_ms4_kmax1_kminNone_a0.7_M4_fFalse_dlTrue_one3_224_epoch03.pt'</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA{}_compf_cls_att_gd_nf4_norm{}_hb_{}_aug7_{}_thm_rf{}_hth{}_ms4_kmax{}_kmin{}_a{}_M{}_f{}_dl{}_one3_224_epoch03.pt'</t>
+  </si>
+  <si>
+    <t>train_cw_aug_gbvs (model_name)</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA{}_compf_cls_att_gd_nf4_norm{}_hb_{}_aug7_{}_thm_rf{}_hth{}_ms4_kmax{}_kmin{}_a{}_M{}_f{}_dl{}_one3_224</t>
+  </si>
+  <si>
+    <t>train_cw_aug_sa_art(checkpoint)</t>
+  </si>
+  <si>
+    <t>basemodel_210428_sgd</t>
+  </si>
+  <si>
+    <t>model.parameters().requires_grad=False</t>
+  </si>
+  <si>
+    <t>basemodel_alt_210509_adam</t>
+  </si>
+  <si>
+    <t>basemodel_alt_210509_adam_2</t>
+  </si>
+  <si>
+    <t>basemodel_210508_adam</t>
+  </si>
+  <si>
+    <t>basemodel_210504_sgd</t>
+  </si>
+  <si>
+    <t>[40] 1.4388</t>
+  </si>
+  <si>
+    <t>[6] 1.3861</t>
+  </si>
+  <si>
+    <t>nips08 do not sub mean</t>
+  </si>
+  <si>
+    <t>resnet50_wildcat_wk_hd_cbA{}_compf_cls_att_gd_nf4_norm{}_hb_{}_aug7_{}_{}_thm_rf{}_hth{}_ms4_fdim{}_34_cw_sa_art_fixf_3_kmax{}_kmin{}_a{}_M{}_f{}_dl{}_one3_224</t>
+  </si>
+  <si>
+    <t>train_cw_aug_sa_art(model_name)</t>
+  </si>
+  <si>
+    <t>_34_cw_sa_art_fixf_sp</t>
+  </si>
+  <si>
+    <t>_ms4_sa_art_ftf_2_4_sp</t>
+  </si>
+  <si>
+    <t>_ms4_sa_art_fixf_kmax</t>
+  </si>
+  <si>
+    <t>_alt_2_compf_cls_att_gd_</t>
+  </si>
+  <si>
+    <t>_aug7_{}_thm_rf{}_hth{}_ms4_kmax{}_kmin{}_a{}_M{}_f{}_dl{}_one3_224</t>
+  </si>
+  <si>
+    <t>[28] 1.4951</t>
+  </si>
+  <si>
+    <t>train_Wildcat_WK_hd_compf_map_cw_alt_alpha</t>
+  </si>
+  <si>
+    <t>[82] 1.6612; [111] 1.7202</t>
+  </si>
+  <si>
+    <t>210424_sgd_2</t>
+  </si>
+  <si>
+    <t>[27] 1.4748</t>
+  </si>
+  <si>
+    <t>sa_sp_alt_210511_sgd</t>
+  </si>
+  <si>
+    <t>sa_sp_alt_210511_adam</t>
+  </si>
+  <si>
+    <t>2-1)</t>
+  </si>
+  <si>
+    <t>2-2)</t>
+  </si>
+  <si>
+    <t>1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,13 +337,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,9 +410,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -499,261 +703,552 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D47"/>
+  <dimension ref="A2:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" t="s">
+        <v>77</v>
+      </c>
+      <c r="D81" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" t="s">
+        <v>86</v>
+      </c>
+      <c r="D82" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E84" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="E85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" t="s">
-        <v>28</v>
+    <row r="88" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>75</v>
+      </c>
+      <c r="C90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>95</v>
+      </c>
+      <c r="B102" t="s">
+        <v>89</v>
+      </c>
+      <c r="C102" t="s">
+        <v>90</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B103" t="s">
+        <v>91</v>
+      </c>
+      <c r="D103" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
train on COCO all.
</commit_message>
<xml_diff>
--- a/model list.xlsx
+++ b/model list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F623F-BF6E-4950-A2A9-449F4148E6E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A9B187-63BD-4826-983E-C6C1858FA686}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>phase</t>
   </si>
@@ -286,9 +286,6 @@
     <t>train_Wildcat_WK_hd_compf_map_cw_alt_alpha</t>
   </si>
   <si>
-    <t>[82] 1.6612; [111] 1.7202</t>
-  </si>
-  <si>
     <t>210424_sgd_2</t>
   </si>
   <si>
@@ -308,6 +305,12 @@
   </si>
   <si>
     <t>1)</t>
+  </si>
+  <si>
+    <t>如果这个成功了，其实何以合成一个alt的步骤，就是nss&lt;prior(或者某个target)的时候，一直用prior。后面超过prior了，就用自己就行了。</t>
+  </si>
+  <si>
+    <t>[82] 1.6612; [111] 1.7202; [133] 1.7278</t>
   </si>
 </sst>
 </file>
@@ -705,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1173,7 @@
         <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -1215,13 +1218,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B102" t="s">
+        <v>88</v>
+      </c>
+      <c r="C102" t="s">
         <v>89</v>
-      </c>
-      <c r="C102" t="s">
-        <v>90</v>
       </c>
       <c r="D102" t="s">
         <v>12</v>
@@ -1229,10 +1232,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D103" t="s">
         <v>16</v>
@@ -1240,10 +1243,15 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>